<commit_message>
update indra script to return Biorecipe reading_output format
</commit_message>
<xml_diff>
--- a/examples/indra_search_paper/CAR_TCELL_reading.xlsx
+++ b/examples/indra_search_paper/CAR_TCELL_reading.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>Regulator Name</t>
   </si>
@@ -22,13 +22,22 @@
     <t>Regulator Type</t>
   </si>
   <si>
+    <t>Regulator Subtype</t>
+  </si>
+  <si>
+    <t>Regulator HGNC ID</t>
+  </si>
+  <si>
+    <t>Regulator Database</t>
+  </si>
+  <si>
     <t>Regulator ID</t>
   </si>
   <si>
-    <t>Regulator Location</t>
-  </si>
-  <si>
-    <t>Regulator Database</t>
+    <t>Regulator Compartment</t>
+  </si>
+  <si>
+    <t>Regulator Compartment ID</t>
   </si>
   <si>
     <t>Regulated Name</t>
@@ -37,13 +46,22 @@
     <t>Regulated Type</t>
   </si>
   <si>
+    <t>Regulated Subtype</t>
+  </si>
+  <si>
+    <t>Regulated HGNC ID</t>
+  </si>
+  <si>
+    <t>Regulated Database</t>
+  </si>
+  <si>
     <t>Regulated ID</t>
   </si>
   <si>
-    <t>Regulated Location</t>
-  </si>
-  <si>
-    <t>Regulated Database</t>
+    <t>Regulated Compartment</t>
+  </si>
+  <si>
+    <t>Regulated Compartment ID</t>
   </si>
   <si>
     <t>Sign</t>
@@ -52,31 +70,34 @@
     <t>Connection Type</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Mechanism</t>
   </si>
   <si>
+    <t>Site</t>
+  </si>
+  <si>
     <t>Cell Line</t>
   </si>
   <si>
     <t>Cell Type</t>
   </si>
   <si>
+    <t>Tissue Type</t>
+  </si>
+  <si>
     <t>Organism</t>
   </si>
   <si>
-    <t>Tissue Type</t>
-  </si>
-  <si>
-    <t>Evidence</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
-    <t>Paper ID</t>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Statements</t>
+  </si>
+  <si>
+    <t>Paper IDs</t>
   </si>
   <si>
     <t>CD8</t>
@@ -109,6 +130,9 @@
     <t>protein</t>
   </si>
   <si>
+    <t>uniprot</t>
+  </si>
+  <si>
     <t>P01730</t>
   </si>
   <si>
@@ -124,9 +148,6 @@
     <t>P33681</t>
   </si>
   <si>
-    <t>uniprot</t>
-  </si>
-  <si>
     <t>IL2</t>
   </si>
   <si>
@@ -151,22 +172,22 @@
     <t>bioprocess</t>
   </si>
   <si>
+    <t>go</t>
+  </si>
+  <si>
     <t>P60568</t>
   </si>
   <si>
     <t>P01579</t>
   </si>
   <si>
-    <t>GO:0008283</t>
+    <t>0008283</t>
   </si>
   <si>
     <t>P15391</t>
   </si>
   <si>
     <t>P10747</t>
-  </si>
-  <si>
-    <t>go</t>
   </si>
   <si>
     <t>positive</t>
@@ -578,13 +599,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,402 +669,423 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>45</v>
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
       </c>
       <c r="N2" t="s">
         <v>53</v>
       </c>
+      <c r="Q2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s">
+        <v>59</v>
+      </c>
       <c r="S2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>60</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
       </c>
       <c r="N3" t="s">
         <v>54</v>
       </c>
+      <c r="Q3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" t="s">
+        <v>59</v>
+      </c>
       <c r="S3" t="s">
-        <v>56</v>
-      </c>
-      <c r="U3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+        <v>61</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" t="s">
+        <v>59</v>
+      </c>
+      <c r="S6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
         <v>47</v>
       </c>
-      <c r="J4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" t="s">
-        <v>53</v>
-      </c>
-      <c r="S4" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" t="s">
-        <v>53</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="Q7" t="s">
         <v>58</v>
       </c>
-      <c r="U5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N6" t="s">
-        <v>53</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="R7" t="s">
         <v>59</v>
-      </c>
-      <c r="U6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" t="s">
-        <v>51</v>
-      </c>
-      <c r="L7" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" t="s">
-        <v>53</v>
       </c>
       <c r="S7" t="s">
         <v>60</v>
       </c>
-      <c r="U7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="AA7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
         <v>30</v>
       </c>
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
       <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" t="s">
+        <v>59</v>
+      </c>
+      <c r="S8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" t="s">
+        <v>59</v>
+      </c>
+      <c r="S10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="K8" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N8" t="s">
-        <v>53</v>
-      </c>
-      <c r="S8" t="s">
-        <v>61</v>
-      </c>
-      <c r="U8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" t="s">
+        <v>59</v>
+      </c>
+      <c r="S11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s">
         <v>50</v>
       </c>
-      <c r="K9" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" t="s">
-        <v>53</v>
-      </c>
-      <c r="S9" t="s">
-        <v>62</v>
-      </c>
-      <c r="U9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" t="s">
-        <v>53</v>
-      </c>
-      <c r="S10" t="s">
-        <v>63</v>
-      </c>
-      <c r="U10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L11" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" t="s">
-        <v>53</v>
-      </c>
-      <c r="S11" t="s">
-        <v>64</v>
-      </c>
-      <c r="U11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" t="s">
-        <v>53</v>
+      <c r="Q12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R12" t="s">
+        <v>59</v>
       </c>
       <c r="S12" t="s">
-        <v>65</v>
-      </c>
-      <c r="U12" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>